<commit_message>
fixed bug in climate proj formatting
</commit_message>
<xml_diff>
--- a/tables/TableS8-9_envi_param_table.xlsx
+++ b/tables/TableS8-9_envi_param_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/aquacast/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C285ADC-F203-4942-9441-9F55187618FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777C8F86-1450-1040-82C5-F6E8AA0ED7E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{BF55C753-D646-E645-A0FE-9B968723D3C6}"/>
+    <workbookView xWindow="17520" yWindow="4600" windowWidth="25600" windowHeight="15540" xr2:uid="{BF55C753-D646-E645-A0FE-9B968723D3C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>Sea surface salinity (psu)</t>
   </si>
@@ -149,6 +149,24 @@
   </si>
   <si>
     <t>Barton et al. (2015)</t>
+  </si>
+  <si>
+    <t>Current velocity</t>
+  </si>
+  <si>
+    <t>Wave height</t>
+  </si>
+  <si>
+    <t>0.04 - 1.6 m/s</t>
+  </si>
+  <si>
+    <t>Froehlich et al. (2017)</t>
+  </si>
+  <si>
+    <t>&lt; 12 m</t>
+  </si>
+  <si>
+    <t>uo / vo (m/s)</t>
   </si>
 </sst>
 </file>
@@ -561,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C3950F-ED25-DB45-8A81-54A0ECFF7DFA}">
   <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -680,6 +698,34 @@
         <v>40</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D18" s="4"/>
     </row>
@@ -705,7 +751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF08F666-4C69-6449-9475-5A25B8B02AF9}">
   <dimension ref="A2:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
a lot of work for revisions
</commit_message>
<xml_diff>
--- a/tables/TableS8-9_envi_param_table.xlsx
+++ b/tables/TableS8-9_envi_param_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/aquacast/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777C8F86-1450-1040-82C5-F6E8AA0ED7E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941D5667-B552-9F49-BB53-26ECFAC5B312}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17520" yWindow="4600" windowWidth="25600" windowHeight="15540" xr2:uid="{BF55C753-D646-E645-A0FE-9B968723D3C6}"/>
+    <workbookView xWindow="19000" yWindow="10800" windowWidth="25600" windowHeight="15540" xr2:uid="{BF55C753-D646-E645-A0FE-9B968723D3C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>Sea surface salinity (psu)</t>
   </si>
@@ -76,9 +76,6 @@
     <t>&lt; 0.1244 mol/m3 (&lt; 1.99 mg/L)</t>
   </si>
   <si>
-    <t>Dissolved oxygen concentration at surface (mol/m3)</t>
-  </si>
-  <si>
     <t>Code (native units)</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>po4 (mol/m3)</t>
   </si>
   <si>
-    <t>Total chlorophyll concentration at surface (mg/m3)</t>
-  </si>
-  <si>
     <t>Bivalves limits</t>
   </si>
   <si>
@@ -151,22 +145,31 @@
     <t>Barton et al. (2015)</t>
   </si>
   <si>
-    <t>Current velocity</t>
-  </si>
-  <si>
-    <t>Wave height</t>
-  </si>
-  <si>
-    <t>0.04 - 1.6 m/s</t>
-  </si>
-  <si>
     <t>Froehlich et al. (2017)</t>
   </si>
   <si>
-    <t>&lt; 12 m</t>
-  </si>
-  <si>
     <t>uo / vo (m/s)</t>
+  </si>
+  <si>
+    <t>Current speed (m/s)</t>
+  </si>
+  <si>
+    <t>Hs (m)</t>
+  </si>
+  <si>
+    <t>&lt; 5 m</t>
+  </si>
+  <si>
+    <t>0.04 - 1.0 m/s</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen concentration (mol/m3)</t>
+  </si>
+  <si>
+    <t>Total chlorophyll concentration (mg/m3)</t>
+  </si>
+  <si>
+    <t>Significant wave height (m)</t>
   </si>
 </sst>
 </file>
@@ -580,7 +583,7 @@
   <dimension ref="A2:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,19 +600,19 @@
   <sheetData>
     <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -627,7 +630,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -644,7 +647,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -652,7 +655,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
@@ -661,7 +664,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -669,61 +672,67 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
@@ -763,10 +772,10 @@
   <sheetData>
     <row r="2" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -774,7 +783,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -782,31 +791,31 @@
         <v>6</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -814,12 +823,12 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>4</v>
@@ -843,18 +852,18 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>